<commit_message>
Add Sri Lanka 40x30mm project
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -117,9 +117,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -142,14 +149,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -165,7 +188,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -181,25 +204,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -547,129 +570,129 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88.875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>59</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>